<commit_message>
Implementing PHP7.4-8.x transformers as PHP8.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgSupportedLangStringGroup.xlsx
+++ b/meta/program/BlancoCgSupportedLangStringGroup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEE3D1C9-B726-0044-B89C-9FF46FBE9292}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97C8696-B778-9A41-BC8C-D8CEEB9443EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="19900" windowHeight="14300"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="19900" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stringGroup" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="デリミタ">#REF!</definedName>
     <definedName name="型">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>説明</t>
     <rPh sb="0" eb="2">
@@ -395,6 +395,30 @@
     <t>TypeScript言語。</t>
     <rPh sb="10" eb="12">
       <t xml:space="preserve">ゲンゴ </t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>php8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>PHP8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>PHP言語（型宣言対応版）。</t>
+    <rPh sb="3" eb="5">
+      <t>ゲンゴ</t>
+    </rPh>
+    <rPh sb="6" eb="9">
+      <t xml:space="preserve">カタセンゲｎ </t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t xml:space="preserve">タイオウ </t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t xml:space="preserve">バｎ </t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
@@ -402,7 +426,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -780,32 +804,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -824,9 +848,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -864,9 +888,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -899,26 +923,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,26 +958,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1143,14 +1133,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1189,74 +1179,74 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="30"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="25" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="30"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="29"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="30"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="31"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="35"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6">
@@ -1443,10 +1433,19 @@
       <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="8"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
+      <c r="A27" s="8">
+        <f>A26+1</f>
+        <v>13</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>54</v>
+      </c>
       <c r="E27" s="15"/>
     </row>
     <row r="28" spans="1:5">
@@ -1485,11 +1484,18 @@
       <c r="E32" s="15"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="16"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="11"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>